<commit_message>
refactored frog pipeline, cleaned up generic pipeline
</commit_message>
<xml_diff>
--- a/02_generic_data_compilation/results/output_results.xlsx
+++ b/02_generic_data_compilation/results/output_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Social Dominance Hierarchy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Territoriality (males)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Territoriality (females)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Group Size During Reproduction</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Group Size Outside of Reproduction</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Group Property</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Age at Maturity</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Avg. life expectancy</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t># offspring/reproductive bout</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t># reproductive bouts/year</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Migratory behavior</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Activity Pattern</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Habitat Complexity</t>
         </is>
       </c>
     </row>
@@ -468,24 +518,50 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Monogamous</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.3 years</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+          <t>Small territories; Large territories (wandering)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>small groups (2-10 individuals)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>small groups</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>&gt;0.3 years</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -495,24 +571,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+          <t>Promiscuous</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -522,22 +608,44 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Monogamous</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Linear</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Small groups (2-10 individuals); 1M:2F and 1M:1F mating setups</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>solitary</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>0.15 years</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>complex (urban/synanthropic environments)</t>
         </is>
       </c>
     </row>
@@ -549,22 +657,919 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Polygynous</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+          <t>Linear; Non-Linear (group-dependent)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>small groups (2-10)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>small groups (2-10 individuals)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>0.25 years</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Urban/sewer environments; high structural complexity</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cavia porcellus</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Promiscuous</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>medium groups (10-100 individuals)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>cooperative</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Female ~0.08 years; Male ~0.17–0.25 years</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>mosaic forest–savanna (open forest and grassland)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Fukomys damarensis</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Monogamous</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>large groups</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2-26 (wild); 1-17 (captive)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>cooperative</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.74 years</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>yearround</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Underground burrow maze with numerous chambers; tunnel system up to 1 km long.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pan troglodytes</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Promiscuous</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Non-Linear</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Large territories</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>large</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>large (community ~110+ individuals); medium (subgroups ~31 individuals)</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10 years</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>29 years</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>multilevel, vertically structured enclosures with shelter and varied structures; higher enclosure complexity linked to better chimpanzee welfare.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Monogamous; Promiscuous</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Non-Linear</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>large groups</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>cooperative</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>forest-dwelling frugivore to savanna predator; savanna habitats</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gorilla gorilla</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Polygynous</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Leipzig Zoo - small group (7); Burgers' Zoo - medium group (12); Vallée des Singes - small group (9)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>7; 12; 9</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>cooperative</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>6.4–8.8 years</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Gorilla gorilla milk microbiomes more similar when individuals are at the same facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hylobates lar</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Monogamous; Polyandrous; Polygynous</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>small groups (2-10)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>6-8 years</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>yearround</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>tropical rainforest; China distribution limited to Lincang, Yunnan.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Macaca mulatta</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Promiscuous</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Large territories</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>large groups (100-1000 or more)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>small groups (2-10)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>4 years</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>low slopes; low EVI values</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Macaca fascicularis</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>medium groups (10-100 individuals)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2 years</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>yes (male migration; female philopatry)</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>associated with intact forest structure; M. fascicularis largely absent from 44% of sites with medium–high forest integrity</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Passer domesticus</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Monogamous</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Mentioned; no hierarchy type provided.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>small groups (2-10)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>large groups (100-1000+)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>seasonal</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Foliage Height Diversity (FHD) – best predictor of Passer domesticus abundance and species richness.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Zonotrichia albicollis</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>seasonal</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Taeniopygia guttata</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Monogamous</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>small groups (2-10 individuals)</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>cooperative</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.21 years</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>habitat heterogeneity/variability -&gt; greater cultural richness (passerines; Taeniopygia guttata)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pipra filicauda</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Polygynous</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Large territories</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>small groups (4-12 territorial males per lek)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>no, they migrate eventually</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Columba livia</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Monogamous</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>large groups</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>large groups</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>interactional</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.5 years</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>urban areas (low complexity)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Coturnix japonica</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Promiscuous</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>medium groups (10-100)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.14 years</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>year-round</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>cage enrichments (nest box, scratcher, tunnel, limestone cubes, sand, feeder) increase environmental complexity for Coturnix japonica</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Anolis carolinensis</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Small territories</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>solitary (no sociality)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>solitary</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>reduced canopy cover; higher impervious surface in urban habitats</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Engystomops putulosus</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dendrobate auratus</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Astatotilap burtoni</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Gasterosteus aculeatus</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Large territories</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>medium groups (10-100)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1.9 years</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>yes (anadromous migrate from sea to rivers to spawn); no (freshwater residents year-round).</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>higher abundance of Gasterosteus aculeatus at coarse-bottom, exposed habitats; lower at simple-structured sandy shores</t>
         </is>
       </c>
     </row>

</xml_diff>